<commit_message>
Stable Version 1.1 GM HeatStakes
</commit_message>
<xml_diff>
--- a/Reportes/EXERCISE 1 -DOOR PANELS/Reporte_EXERCISE 1 -DOOR PANELS.xlsx
+++ b/Reportes/EXERCISE 1 -DOOR PANELS/Reporte_EXERCISE 1 -DOOR PANELS.xlsx
@@ -468,7 +468,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-376</t>
+          <t>MERGED-GRP1+GRP2-88</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -492,7 +492,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-760</t>
+          <t>MERGED-GRP1+GRP2-80</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -516,7 +516,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-16</t>
+          <t>MERGED-GRP1+GRP2-336</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -540,7 +540,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-400</t>
+          <t>MERGED-GRP1+GRP2-720</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -564,7 +564,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-848</t>
+          <t>MERGED-GRP1+GRP2-168</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -588,7 +588,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-296</t>
+          <t>MERGED-GRP1+GRP2-616</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -612,7 +612,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-808</t>
+          <t>MERGED-GRP1+GRP2-128</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -636,7 +636,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-128</t>
+          <t>MERGED-GRP1+GRP2-448</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -660,7 +660,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-576</t>
+          <t>MERGED-GRP1+GRP2-896</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -684,7 +684,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-24</t>
+          <t>MERGED-GRP1+GRP2-344</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -708,7 +708,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-344</t>
+          <t>MERGED-GRP1+GRP2-664</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -732,7 +732,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-728</t>
+          <t>MERGED-GRP1+GRP2-48</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -756,7 +756,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-112</t>
+          <t>MERGED-GRP1+GRP2-432</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -780,7 +780,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-496</t>
+          <t>MERGED-GRP1+GRP2-816</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -804,7 +804,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-880</t>
+          <t>MERGED-GRP1+GRP2-200</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -828,7 +828,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-200</t>
+          <t>MERGED-GRP1+GRP2-520</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -852,7 +852,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-712</t>
+          <t>MERGED-GRP1+GRP2-32</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -876,7 +876,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-32</t>
+          <t>MERGED-GRP1+GRP2-352</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -900,7 +900,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-480</t>
+          <t>MERGED-GRP1+GRP2-800</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -924,7 +924,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-800</t>
+          <t>MERGED-GRP1+GRP2-120</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -948,7 +948,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-984</t>
+          <t>MERGED-GRP1+GRP2-632</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -972,7 +972,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-368</t>
+          <t>MERGED-GRP1+GRP2-688</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -996,7 +996,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-816</t>
+          <t>MERGED-GRP1+GRP2-136</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1020,7 +1020,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-200</t>
+          <t>MERGED-GRP1+GRP2-520</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1044,7 +1044,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-584</t>
+          <t>MERGED-GRP1+GRP2-904</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1068,7 +1068,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-32</t>
+          <t>MERGED-GRP1+GRP2-352</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1092,7 +1092,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-480</t>
+          <t>MERGED-GRP1+GRP2-800</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1116,7 +1116,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-800</t>
+          <t>MERGED-GRP1+GRP2-120</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1140,7 +1140,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-248</t>
+          <t>MERGED-GRP1+GRP2-568</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1164,7 +1164,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-632</t>
+          <t>MERGED-GRP1+GRP2-952</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1188,7 +1188,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-16</t>
+          <t>MERGED-GRP1+GRP2-336</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1212,7 +1212,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-400</t>
+          <t>MERGED-GRP1+GRP2-720</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1236,7 +1236,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-848</t>
+          <t>MERGED-GRP1+GRP2-168</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1260,7 +1260,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-232</t>
+          <t>MERGED-GRP1+GRP2-552</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1284,7 +1284,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-552</t>
+          <t>MERGED-GRP1+GRP2-872</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1308,7 +1308,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-64</t>
+          <t>MERGED-GRP1+GRP2-384</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1332,7 +1332,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-448</t>
+          <t>MERGED-GRP1+GRP2-768</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1356,7 +1356,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-832</t>
+          <t>MERGED-GRP1+GRP2-152</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1380,7 +1380,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-216</t>
+          <t>MERGED-GRP1+GRP2-536</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1404,7 +1404,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-600</t>
+          <t>MERGED-GRP1+GRP2-920</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1428,7 +1428,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-48</t>
+          <t>MERGED-GRP1+GRP2-368</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1452,7 +1452,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-432</t>
+          <t>MERGED-GRP1+GRP2-752</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1476,7 +1476,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-752</t>
+          <t>MERGED-GRP1+GRP2-72</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1500,7 +1500,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-264</t>
+          <t>MERGED-GRP1+GRP2-584</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1524,7 +1524,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-648</t>
+          <t>MERGED-GRP1+GRP2-968</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1548,7 +1548,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-968</t>
+          <t>MERGED-GRP1+GRP2-288</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1572,7 +1572,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>MERGED-GRP1+GRP2-416</t>
+          <t>MERGED-GRP1+GRP2-736</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">

</xml_diff>